<commit_message>
send from HRM Project 2023 dec
</commit_message>
<xml_diff>
--- a/testdata/New Microsoft Excel Worksheet.xlsx
+++ b/testdata/New Microsoft Excel Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtas6\IdeaProjects\com.OrangeHRM\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8143BD-B391-4B44-A1D0-6D7AAC3F52F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5857E24D-ADCF-45DD-BA43-FEFAC875912D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>BookName</t>
   </si>
@@ -48,13 +48,7 @@
     <t>Java</t>
   </si>
   <si>
-    <t>2nd May</t>
-  </si>
-  <si>
     <t>Python</t>
-  </si>
-  <si>
-    <t>3rd May</t>
   </si>
   <si>
     <t>Ruby</t>
@@ -64,6 +58,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -95,7 +92,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,19 +376,20 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.6328125" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -419,8 +417,8 @@
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
+      <c r="B3" s="1">
+        <v>45048</v>
       </c>
       <c r="C3">
         <v>300</v>
@@ -431,10 +429,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45049</v>
       </c>
       <c r="C4">
         <v>400</v>
@@ -445,7 +443,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
         <v>45107</v>
@@ -459,5 +457,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>